<commit_message>
working design 3 track
working design 3 track
</commit_message>
<xml_diff>
--- a/UPVC.xlsx
+++ b/UPVC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Documents\GitHub\PhoenixTools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38332A47-B837-4D6E-8882-D4F96C8B8A0D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A181D2C-2C70-4252-9E4C-FC942B7967F8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9525" xr2:uid="{3A4AF54F-C135-40A6-864C-09529CEE8C41}"/>
   </bookViews>
@@ -704,8 +704,8 @@
   <dimension ref="B3:Y15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="5" topLeftCell="R1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E4" sqref="E4:E8"/>
+      <pane xSplit="5" topLeftCell="S1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="U4" sqref="U4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -878,7 +878,7 @@
         <v>421.47436725429009</v>
       </c>
       <c r="V4">
-        <f>SUM(K4:U4)+F4+G4</f>
+        <f t="shared" ref="V4:V15" si="0">SUM(K4:U4)+F4+G4</f>
         <v>5820.8250928120133</v>
       </c>
       <c r="W4">
@@ -935,7 +935,7 @@
         <v>421.47436725429009</v>
       </c>
       <c r="V5">
-        <f>SUM(K5:U5)+F5+G5</f>
+        <f t="shared" si="0"/>
         <v>1848.5632908611542</v>
       </c>
       <c r="W5">
@@ -943,11 +943,11 @@
         <v>219.29723780163502</v>
       </c>
       <c r="X5">
-        <f t="shared" ref="X5:X8" si="0">W5*115%</f>
+        <f t="shared" ref="X5:X8" si="1">W5*115%</f>
         <v>252.19182347188024</v>
       </c>
       <c r="Y5">
-        <f t="shared" ref="Y5:Y8" si="1">X5*118%</f>
+        <f t="shared" ref="Y5:Y8" si="2">X5*118%</f>
         <v>297.58635169681867</v>
       </c>
     </row>
@@ -1018,7 +1018,7 @@
         <v>421.47436725429009</v>
       </c>
       <c r="V6">
-        <f>SUM(K6:U6)+F6+G6</f>
+        <f t="shared" si="0"/>
         <v>3013.0724597628705</v>
       </c>
       <c r="W6">
@@ -1026,11 +1026,11 @@
         <v>357.44433040989412</v>
       </c>
       <c r="X6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>411.06097997137823</v>
       </c>
       <c r="Y6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>485.05195636622631</v>
       </c>
     </row>
@@ -1100,23 +1100,23 @@
         <v>100</v>
       </c>
       <c r="U7">
-        <f t="shared" ref="U7:U15" si="2">MIN(E7*D7/92903.04*50,2000)</f>
+        <f t="shared" ref="U7:U15" si="3">MIN(E7*D7/92903.04*50,2000)</f>
         <v>421.47436725429009</v>
       </c>
       <c r="V7">
-        <f>SUM(K7:U7)+F7+G7</f>
+        <f t="shared" si="0"/>
         <v>4206.6683118611545</v>
       </c>
       <c r="W7">
-        <f t="shared" ref="W7:W15" si="3">V7/(E7*D7)*92903.04</f>
+        <f t="shared" ref="W7:W15" si="4">V7/(E7*D7)*92903.04</f>
         <v>499.04201046265825</v>
       </c>
       <c r="X7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>573.89831203205699</v>
       </c>
       <c r="Y7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>677.20000819782717</v>
       </c>
     </row>
@@ -1191,23 +1191,23 @@
         <v>100</v>
       </c>
       <c r="U8">
+        <f t="shared" si="3"/>
+        <v>421.47436725429009</v>
+      </c>
+      <c r="V8">
+        <f t="shared" si="0"/>
+        <v>4984.7689378120131</v>
+      </c>
+      <c r="W8">
+        <f t="shared" si="4"/>
+        <v>591.3490030586521</v>
+      </c>
+      <c r="X8">
+        <f t="shared" si="1"/>
+        <v>680.05135351744991</v>
+      </c>
+      <c r="Y8">
         <f t="shared" si="2"/>
-        <v>421.47436725429009</v>
-      </c>
-      <c r="V8">
-        <f>SUM(K8:U8)+F8+G8</f>
-        <v>4984.7689378120131</v>
-      </c>
-      <c r="W8">
-        <f t="shared" si="3"/>
-        <v>591.3490030586521</v>
-      </c>
-      <c r="X8">
-        <f t="shared" si="0"/>
-        <v>680.05135351744991</v>
-      </c>
-      <c r="Y8">
-        <f t="shared" si="1"/>
         <v>802.46059715059084</v>
       </c>
     </row>
@@ -1221,15 +1221,15 @@
         <v>0</v>
       </c>
       <c r="U9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="V9">
-        <f>SUM(K9:U9)+F9+G9</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="W9" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1243,15 +1243,15 @@
         <v>0</v>
       </c>
       <c r="U10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="V10">
-        <f>SUM(K10:U10)+F10+G10</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="W10" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1265,15 +1265,15 @@
         <v>0</v>
       </c>
       <c r="U11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="V11">
-        <f>SUM(K11:U11)+F11+G11</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="W11" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1287,15 +1287,15 @@
         <v>0</v>
       </c>
       <c r="U12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="V12">
-        <f>SUM(K12:U12)+F12+G12</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="W12" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1309,43 +1309,43 @@
         <v>0</v>
       </c>
       <c r="U13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="V13">
-        <f>SUM(K13:U13)+F13+G13</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="W13" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="14" spans="2:25" x14ac:dyDescent="0.25">
       <c r="U14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="V14">
-        <f>SUM(K14:U14)+F14+G14</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="W14" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="15" spans="2:25" x14ac:dyDescent="0.25">
       <c r="U15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="V15">
-        <f>SUM(K15:U15)+F15+G15</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="W15" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1359,7 +1359,7 @@
   <dimension ref="B2:K23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:XFD13"/>
+      <selection activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>